<commit_message>
somewhat fixed the order_processor.py validator
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\BCIT Work Synced Folder\My Courses\COMP3522 OOP 2\Winter 2020\Assignments\Assignment 2 Supply Chain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickmcgrath/PycharmProjects/3522_A00931408/Assignments/COMP3522_Assignment2_A00989893_A00931408/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F959E200-ABA9-4C24-84DC-7F0EB85250A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E841C8AA-1CE6-7244-B680-732B6069634C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
+    <workbookView xWindow="-28800" yWindow="3600" windowWidth="28800" windowHeight="18000" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="93">
   <si>
     <t>name</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>Sea Salt</t>
+  </si>
+  <si>
+    <t>Tarantula s</t>
   </si>
 </sst>
 </file>
@@ -663,34 +666,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC969572-FB28-418E-B89D-F0DD002AE5AA}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T14" sqref="T14"/>
+      <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="56.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="56.83203125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" customWidth="1"/>
-    <col min="18" max="18" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9.5" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="14" max="14" width="10.1640625" customWidth="1"/>
+    <col min="15" max="15" width="14.83203125" customWidth="1"/>
+    <col min="16" max="16" width="13.5" customWidth="1"/>
+    <col min="17" max="17" width="8.5" customWidth="1"/>
+    <col min="18" max="18" width="12.5" customWidth="1"/>
     <col min="22" max="22" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -764,7 +767,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -799,7 +802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -834,7 +837,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -869,7 +872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -904,7 +907,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -942,10 +945,10 @@
         <v>34</v>
       </c>
       <c r="O6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -977,7 +980,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1047,7 +1050,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1079,7 +1082,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1114,7 +1117,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1155,7 +1158,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1196,7 +1199,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1260,13 +1263,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G18" s="1"/>
     </row>
   </sheetData>

</xml_diff>